<commit_message>
Fixed C3DC phs000437 testcases
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC03_C3DC_phs000467_Race-HispOrLatino.xlsx
+++ b/InputFiles/C3DC/TC03_C3DC_phs000467_Race-HispOrLatino.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-27-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE175BA-DD72-7144-B8C6-E053C5200057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E7E551-4B64-504C-B8B1-DA688F6E906B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-   std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino');</t>
+   std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino', 'Black or African American;Hispanic or Latino', 'Asian;Hispanic or Latino');</t>
   </si>
   <si>
     <t>SELECT DISTINCT
@@ -117,7 +117,7 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino')</t>
+    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino', 'Black or African American;Hispanic or Latino', 'Asian;Hispanic or Latino')</t>
   </si>
   <si>
     <t>SELECT DISTINCT
@@ -140,7 +140,7 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino')
+    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino', 'Black or African American;Hispanic or Latino', 'Asian;Hispanic or Latino')
 ORDER BY 
     prt.participant_id ASC
 LIMIT 100;</t>
@@ -177,7 +177,7 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino') AND dgn.diagnosis_id IS NOT NULL
+    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino', 'Black or African American;Hispanic or Latino', 'Asian;Hispanic or Latino') AND dgn.diagnosis_id IS NOT NULL
 ORDER BY 
     prt.participant_id ASC
 LIMIT 100;</t>
@@ -218,7 +218,7 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino')
+    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino', 'Black or African American;Hispanic or Latino', 'Asian;Hispanic or Latino')
 ORDER BY 
     trt.treatment_id ASC
 LIMIT 100;</t>
@@ -253,7 +253,7 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino')
+    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino', 'Black or African American;Hispanic or Latino', 'Asian;Hispanic or Latino')
 ORDER BY 
     prt.participant_id ASC
 LIMIT 100;</t>
@@ -288,7 +288,7 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino') AND srv.survival_id IS NOT NULL
+    std.dbgap_accession = 'phs000467' AND prt.race IN ('Hispanic or Latino;White', 'Hispanic or Latino', 'Black or African American;Hispanic or Latino', 'Asian;Hispanic or Latino') AND srv.survival_id IS NOT NULL
 ORDER BY 
     prt.participant_id ASC
 LIMIT 100;</t>
@@ -683,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>